<commit_message>
Adding energy chart images
</commit_message>
<xml_diff>
--- a/Energy Charts.xlsx
+++ b/Energy Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gux215/Desktop/IAC-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB116CF6-D637-CF46-864D-C3E1C5E3B2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D35DC58-AB86-E949-9A2B-E14281BEFCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="3" r:id="rId1"/>
@@ -10002,7 +10002,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8686800" cy="5486400"/>
+    <xdr:ext cx="8229600" cy="5486400"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 18" descr="Total">
@@ -10234,7 +10234,7 @@
   </sheetPr>
   <dimension ref="A1:W985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -21161,8 +21161,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>